<commit_message>
Figuring out the data
</commit_message>
<xml_diff>
--- a/Data/MSFT.xlsx
+++ b/Data/MSFT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d3073ee5e3651c0a/WUR/Master/Thesis/GitHub/Thesis_Bas/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="8_{85726988-59C3-4F0C-AE9F-F992B21FE08B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7201B1BC-45F6-4C10-AA72-431A007DD25A}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="8_{85726988-59C3-4F0C-AE9F-F992B21FE08B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FB994D91-00C9-4DD4-8061-229324DEEE52}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -568,6 +568,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -869,11 +873,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B162"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" topLeftCell="A123" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
Start working on Predict function
</commit_message>
<xml_diff>
--- a/Data/MSFT.xlsx
+++ b/Data/MSFT.xlsx
@@ -1,21 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d3073ee5e3651c0a/WUR/Master/Thesis/GitHub/Thesis_Bas/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{85726988-59C3-4F0C-AE9F-F992B21FE08B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FB994D91-00C9-4DD4-8061-229324DEEE52}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="8_{85726988-59C3-4F0C-AE9F-F992B21FE08B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AA269D9D-1CA3-4D68-8055-15D7B405006C}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MSFT" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -871,10 +884,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B162"/>
+  <dimension ref="A1:C163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A123" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -882,7 +895,7 @@
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -890,1292 +903,1940 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>44692</v>
       </c>
       <c r="B2">
         <v>257.45593300000002</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <v>1.415E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>44693</v>
       </c>
       <c r="B3">
         <v>252.31770299999999</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <f>(B3-B2)/B2</f>
+        <v>-1.9957706703927547E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>44694</v>
       </c>
       <c r="B4">
         <v>258.01919600000002</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <f t="shared" ref="C4:C67" si="0">(B4-B3)/B3</f>
+        <v>2.2596484242724847E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>44697</v>
       </c>
       <c r="B5">
         <v>258.39468399999998</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>1.455271568243944E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>44698</v>
       </c>
       <c r="B6">
         <v>263.65145899999999</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>2.0343975033170595E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>44699</v>
       </c>
       <c r="B7">
         <v>251.64750699999999</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>-4.5529624776322587E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>44700</v>
       </c>
       <c r="B8">
         <v>250.716522</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>-3.6995597973477744E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>44701</v>
       </c>
       <c r="B9">
         <v>250.14205899999999</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>-2.29128497562681E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>44704</v>
       </c>
       <c r="B10">
         <v>258.15460200000001</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>3.2031970281335302E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>44705</v>
       </c>
       <c r="B11">
         <v>257.13445999999999</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>-3.9516707898936514E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>44706</v>
       </c>
       <c r="B12">
         <v>260.00674400000003</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>1.1170358107583232E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>44707</v>
       </c>
       <c r="B13">
         <v>263.35437000000002</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>1.2875150653784544E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>44708</v>
       </c>
       <c r="B14">
         <v>270.62408399999998</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>2.7604303661260546E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>44712</v>
       </c>
       <c r="B15">
         <v>269.26721199999997</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>-5.0138626981921161E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>44713</v>
       </c>
       <c r="B16">
         <v>269.81195100000002</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>2.0230424490006219E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>44714</v>
       </c>
       <c r="B17">
         <v>271.951233</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>7.9287888919345167E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>44715</v>
       </c>
       <c r="B18">
         <v>267.43490600000001</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>-1.6607120880382218E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>44718</v>
       </c>
       <c r="B19">
         <v>266.17709400000001</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>-4.7032454319930889E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>44719</v>
       </c>
       <c r="B20">
         <v>269.89117399999998</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>1.3953417043466435E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>44720</v>
       </c>
       <c r="B21">
         <v>267.821167</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>-7.6697839700381448E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>44721</v>
       </c>
       <c r="B22">
         <v>262.25500499999998</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>-2.0783129512687171E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>44722</v>
       </c>
       <c r="B23">
         <v>250.56796299999999</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>-4.4563656659288513E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>44725</v>
       </c>
       <c r="B24">
         <v>239.94068899999999</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>-4.2412740530600075E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>44726</v>
       </c>
       <c r="B25">
         <v>242.149338</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C25">
+        <f t="shared" si="0"/>
+        <v>9.2049789854525606E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>44727</v>
       </c>
       <c r="B26">
         <v>249.34973099999999</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C26">
+        <f t="shared" si="0"/>
+        <v>2.973534042864074E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>44728</v>
       </c>
       <c r="B27">
         <v>242.62472500000001</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C27">
+        <f t="shared" si="0"/>
+        <v>-2.6970175476146711E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>44729</v>
       </c>
       <c r="B28">
         <v>245.279068</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C28">
+        <f t="shared" si="0"/>
+        <v>1.0940117500390707E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>44733</v>
       </c>
       <c r="B29">
         <v>251.31079099999999</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C29">
+        <f t="shared" si="0"/>
+        <v>2.459126679330011E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>44734</v>
       </c>
       <c r="B30">
         <v>250.70661899999999</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C30">
+        <f t="shared" si="0"/>
+        <v>-2.4040829985689134E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>44735</v>
       </c>
       <c r="B31">
         <v>256.38174400000003</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C31">
+        <f t="shared" si="0"/>
+        <v>2.2636518423951292E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>44736</v>
       </c>
       <c r="B32">
         <v>265.13717700000001</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C32">
+        <f t="shared" si="0"/>
+        <v>3.4149986123816915E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>44739</v>
       </c>
       <c r="B33">
         <v>262.35403400000001</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C33">
+        <f t="shared" si="0"/>
+        <v>-1.049699265674838E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>44740</v>
       </c>
       <c r="B34">
         <v>254.02453600000001</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C34">
+        <f t="shared" si="0"/>
+        <v>-3.174907537347034E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>44741</v>
       </c>
       <c r="B35">
         <v>257.768372</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C35">
+        <f t="shared" si="0"/>
+        <v>1.4738088134919327E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>44742</v>
       </c>
       <c r="B36">
         <v>254.371185</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C36">
+        <f t="shared" si="0"/>
+        <v>-1.3179223555013966E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>44743</v>
       </c>
       <c r="B37">
         <v>257.09481799999998</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C37">
+        <f t="shared" si="0"/>
+        <v>1.0707317340208869E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>44747</v>
       </c>
       <c r="B38">
         <v>260.33355699999998</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C38">
+        <f t="shared" si="0"/>
+        <v>1.2597449552639408E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>44748</v>
       </c>
       <c r="B39">
         <v>263.66137700000002</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C39">
+        <f t="shared" si="0"/>
+        <v>1.2782908351688336E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>44749</v>
       </c>
       <c r="B40">
         <v>265.830444</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C40">
+        <f t="shared" si="0"/>
+        <v>8.2267149807079398E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>44750</v>
       </c>
       <c r="B41">
         <v>265.09750400000001</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C41">
+        <f t="shared" si="0"/>
+        <v>-2.7571710334275521E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>44753</v>
       </c>
       <c r="B42">
         <v>261.97769199999999</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C42">
+        <f t="shared" si="0"/>
+        <v>-1.1768545357560304E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>44754</v>
       </c>
       <c r="B43">
         <v>251.241455</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C43">
+        <f t="shared" si="0"/>
+        <v>-4.0981493187595489E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>44755</v>
       </c>
       <c r="B44">
         <v>250.30053699999999</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C44">
+        <f t="shared" si="0"/>
+        <v>-3.7450746334835969E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>44756</v>
       </c>
       <c r="B45">
         <v>251.64750699999999</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C45">
+        <f t="shared" si="0"/>
+        <v>5.3814107478323105E-3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>44757</v>
       </c>
       <c r="B46">
         <v>254.26225299999999</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C46">
+        <f t="shared" si="0"/>
+        <v>1.0390510246540995E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>44760</v>
       </c>
       <c r="B47">
         <v>251.81590299999999</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C47">
+        <f t="shared" si="0"/>
+        <v>-9.6213652287584963E-3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>44761</v>
       </c>
       <c r="B48">
         <v>257.04538000000002</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C48">
+        <f t="shared" si="0"/>
+        <v>2.0767064103969762E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>44762</v>
       </c>
       <c r="B49">
         <v>259.75912499999998</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C49">
+        <f t="shared" si="0"/>
+        <v>1.0557454874310365E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>44763</v>
       </c>
       <c r="B50">
         <v>262.30450400000001</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C50">
+        <f t="shared" si="0"/>
+        <v>9.7989974365675341E-3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>44764</v>
       </c>
       <c r="B51">
         <v>257.86740099999997</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C51">
+        <f t="shared" si="0"/>
+        <v>-1.6915847544882553E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>44767</v>
       </c>
       <c r="B52">
         <v>256.35205100000002</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C52">
+        <f t="shared" si="0"/>
+        <v>-5.8764698217901356E-3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>44768</v>
       </c>
       <c r="B53">
         <v>249.488373</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C53">
+        <f t="shared" si="0"/>
+        <v>-2.6774422023251223E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>44769</v>
       </c>
       <c r="B54">
         <v>266.167145</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C54">
+        <f t="shared" si="0"/>
+        <v>6.685190095010965E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>44770</v>
       </c>
       <c r="B55">
         <v>273.76376299999998</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C55">
+        <f t="shared" si="0"/>
+        <v>2.854078026797777E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>44771</v>
       </c>
       <c r="B56">
         <v>278.052277</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C56">
+        <f t="shared" si="0"/>
+        <v>1.5665016994962991E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>44774</v>
       </c>
       <c r="B57">
         <v>275.34845000000001</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C57">
+        <f t="shared" si="0"/>
+        <v>-9.7241678046031243E-3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>44775</v>
       </c>
       <c r="B58">
         <v>272.188965</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C58">
+        <f t="shared" si="0"/>
+        <v>-1.147449713263328E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>44776</v>
       </c>
       <c r="B59">
         <v>279.76568600000002</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C59">
+        <f t="shared" si="0"/>
+        <v>2.7836253391095488E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>44777</v>
       </c>
       <c r="B60">
         <v>280.93441799999999</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C60">
+        <f t="shared" si="0"/>
+        <v>4.1775387707839806E-3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>44778</v>
       </c>
       <c r="B61">
         <v>280.20150799999999</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C61">
+        <f t="shared" si="0"/>
+        <v>-2.6088295098110905E-3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>44781</v>
       </c>
       <c r="B62">
         <v>277.63629200000003</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C62">
+        <f t="shared" si="0"/>
+        <v>-9.1548971963418702E-3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>44782</v>
       </c>
       <c r="B63">
         <v>279.597351</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C63">
+        <f t="shared" si="0"/>
+        <v>7.063410139478369E-3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>44783</v>
       </c>
       <c r="B64">
         <v>286.39166299999999</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C64">
+        <f t="shared" si="0"/>
+        <v>2.4300344676727609E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>44784</v>
       </c>
       <c r="B65">
         <v>284.272156</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C65">
+        <f t="shared" si="0"/>
+        <v>-7.4007287006814812E-3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>44785</v>
       </c>
       <c r="B66">
         <v>289.11535600000002</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C66">
+        <f t="shared" si="0"/>
+        <v>1.7037194455302281E-2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>44788</v>
       </c>
       <c r="B67">
         <v>290.66043100000002</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C67">
+        <f t="shared" si="0"/>
+        <v>5.3441471299781008E-3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>44789</v>
       </c>
       <c r="B68">
         <v>289.90768400000002</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C68">
+        <f t="shared" ref="C68:C131" si="1">(B68-B67)/B67</f>
+        <v>-2.5897814759656755E-3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>44790</v>
       </c>
       <c r="B69">
         <v>289.14343300000002</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C69">
+        <f t="shared" si="1"/>
+        <v>-2.6361874561420784E-3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>44791</v>
       </c>
       <c r="B70">
         <v>288.00201399999997</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C70">
+        <f t="shared" si="1"/>
+        <v>-3.9475874937129965E-3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>44792</v>
       </c>
       <c r="B71">
         <v>284.01205399999998</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C71">
+        <f t="shared" si="1"/>
+        <v>-1.3853930896469345E-2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>44795</v>
       </c>
       <c r="B72">
         <v>275.67483499999997</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C72">
+        <f t="shared" si="1"/>
+        <v>-2.935515898913222E-2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>44796</v>
       </c>
       <c r="B73">
         <v>274.37460299999998</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C73">
+        <f t="shared" si="1"/>
+        <v>-4.7165422262789936E-3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>44797</v>
       </c>
       <c r="B74">
         <v>273.72946200000001</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C74">
+        <f t="shared" si="1"/>
+        <v>-2.3513145639065106E-3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>44798</v>
       </c>
       <c r="B75">
         <v>276.76663200000002</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C75">
+        <f t="shared" si="1"/>
+        <v>1.1095517368897627E-2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>44799</v>
       </c>
       <c r="B76">
         <v>266.08700599999997</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C76">
+        <f t="shared" si="1"/>
+        <v>-3.8587115516150954E-2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>44802</v>
       </c>
       <c r="B77">
         <v>263.24838299999999</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C77">
+        <f t="shared" si="1"/>
+        <v>-1.0668025630684065E-2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>44803</v>
       </c>
       <c r="B78">
         <v>261.00524899999999</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C78">
+        <f t="shared" si="1"/>
+        <v>-8.5209792152835286E-3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>44804</v>
       </c>
       <c r="B79">
         <v>259.516479</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C79">
+        <f t="shared" si="1"/>
+        <v>-5.7039849033840243E-3</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>44805</v>
       </c>
       <c r="B80">
         <v>258.45443699999998</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C80">
+        <f t="shared" si="1"/>
+        <v>-4.0923875204087502E-3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>44806</v>
       </c>
       <c r="B81">
         <v>254.14686599999999</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C81">
+        <f t="shared" si="1"/>
+        <v>-1.6666655252662567E-2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>44810</v>
       </c>
       <c r="B82">
         <v>251.35786400000001</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C82">
+        <f t="shared" si="1"/>
+        <v>-1.0973977542575647E-2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>44811</v>
       </c>
       <c r="B83">
         <v>256.16171300000002</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C83">
+        <f t="shared" si="1"/>
+        <v>1.9111592227725224E-2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>44812</v>
       </c>
       <c r="B84">
         <v>256.58846999999997</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C84">
+        <f t="shared" si="1"/>
+        <v>1.6659671541154641E-3</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>44813</v>
       </c>
       <c r="B85">
         <v>262.48413099999999</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C85">
+        <f t="shared" si="1"/>
+        <v>2.2977108051659603E-2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>44816</v>
       </c>
       <c r="B86">
         <v>264.65774499999998</v>
       </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C86">
+        <f t="shared" si="1"/>
+        <v>8.280934895831803E-3</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>44817</v>
       </c>
       <c r="B87">
         <v>250.10728499999999</v>
       </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C87">
+        <f t="shared" si="1"/>
+        <v>-5.4978402389093087E-2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>44818</v>
       </c>
       <c r="B88">
         <v>250.335556</v>
       </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C88">
+        <f t="shared" si="1"/>
+        <v>9.1269232721472536E-4</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>44819</v>
       </c>
       <c r="B89">
         <v>243.54667699999999</v>
       </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C89">
+        <f t="shared" si="1"/>
+        <v>-2.7119116071550015E-2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>44820</v>
       </c>
       <c r="B90">
         <v>242.91145299999999</v>
       </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C90">
+        <f t="shared" si="1"/>
+        <v>-2.6082228171809291E-3</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>44823</v>
       </c>
       <c r="B91">
         <v>242.69309999999999</v>
       </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C91">
+        <f t="shared" si="1"/>
+        <v>-8.9889956732508436E-4</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>44824</v>
       </c>
       <c r="B92">
         <v>240.638565</v>
       </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C92">
+        <f t="shared" si="1"/>
+        <v>-8.4655682423603607E-3</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>44825</v>
       </c>
       <c r="B93">
         <v>237.16471899999999</v>
       </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C93">
+        <f t="shared" si="1"/>
+        <v>-1.4435948784850878E-2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>44826</v>
       </c>
       <c r="B94">
         <v>239.17953499999999</v>
       </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C94">
+        <f t="shared" si="1"/>
+        <v>8.4954288668880641E-3</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>44827</v>
       </c>
       <c r="B95">
         <v>236.14241000000001</v>
       </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C95">
+        <f t="shared" si="1"/>
+        <v>-1.2698097268229805E-2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>44830</v>
       </c>
       <c r="B96">
         <v>235.67591899999999</v>
       </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C96">
+        <f t="shared" si="1"/>
+        <v>-1.9754647206320078E-3</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>44831</v>
       </c>
       <c r="B97">
         <v>234.64369199999999</v>
       </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C97">
+        <f t="shared" si="1"/>
+        <v>-4.3798577486400129E-3</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>44832</v>
       </c>
       <c r="B98">
         <v>239.26887500000001</v>
       </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C98">
+        <f t="shared" si="1"/>
+        <v>1.9711516472388363E-2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>44833</v>
       </c>
       <c r="B99">
         <v>235.72554</v>
       </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C99">
+        <f t="shared" si="1"/>
+        <v>-1.4809009320581346E-2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>44834</v>
       </c>
       <c r="B100">
         <v>231.159897</v>
       </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C100">
+        <f t="shared" si="1"/>
+        <v>-1.9368469789060594E-2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>44837</v>
       </c>
       <c r="B101">
         <v>238.94134500000001</v>
       </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C101">
+        <f t="shared" si="1"/>
+        <v>3.3662620986546002E-2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>44838</v>
       </c>
       <c r="B102">
         <v>247.02053799999999</v>
       </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C102">
+        <f t="shared" si="1"/>
+        <v>3.3812453010172744E-2</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>44839</v>
       </c>
       <c r="B103">
         <v>247.33812</v>
       </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C103">
+        <f t="shared" si="1"/>
+        <v>1.2856501834678047E-3</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>44840</v>
       </c>
       <c r="B104">
         <v>244.946136</v>
       </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C104">
+        <f t="shared" si="1"/>
+        <v>-9.6709071775915815E-3</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>44841</v>
       </c>
       <c r="B105">
         <v>232.48989900000001</v>
       </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C105">
+        <f t="shared" si="1"/>
+        <v>-5.0852963853244809E-2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>44844</v>
       </c>
       <c r="B106">
         <v>227.53718599999999</v>
       </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C106">
+        <f t="shared" si="1"/>
+        <v>-2.1302916906510493E-2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>44845</v>
       </c>
       <c r="B107">
         <v>223.725876</v>
       </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C107">
+        <f t="shared" si="1"/>
+        <v>-1.6750273074045981E-2</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>44846</v>
       </c>
       <c r="B108">
         <v>224.06333900000001</v>
       </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C108">
+        <f t="shared" si="1"/>
+        <v>1.5083771534769356E-3</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>44847</v>
       </c>
       <c r="B109">
         <v>232.48989900000001</v>
       </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C109">
+        <f t="shared" si="1"/>
+        <v>3.7607937280627578E-2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>44848</v>
       </c>
       <c r="B110">
         <v>226.85232500000001</v>
       </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C110">
+        <f t="shared" si="1"/>
+        <v>-2.424868359549677E-2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>44851</v>
       </c>
       <c r="B111">
         <v>235.75531000000001</v>
       </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C111">
+        <f t="shared" si="1"/>
+        <v>3.9245729573192605E-2</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>44852</v>
       </c>
       <c r="B112">
         <v>236.718063</v>
       </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C112">
+        <f t="shared" si="1"/>
+        <v>4.0836959303270507E-3</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>44853</v>
       </c>
       <c r="B113">
         <v>234.713165</v>
       </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C113">
+        <f t="shared" si="1"/>
+        <v>-8.4695606857850859E-3</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>44854</v>
       </c>
       <c r="B114">
         <v>234.38561999999999</v>
       </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C114">
+        <f t="shared" si="1"/>
+        <v>-1.3955118367562163E-3</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>44855</v>
       </c>
       <c r="B115">
         <v>240.311035</v>
       </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C115">
+        <f t="shared" si="1"/>
+        <v>2.5280625150979893E-2</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>44858</v>
       </c>
       <c r="B116">
         <v>245.40269499999999</v>
       </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C116">
+        <f t="shared" si="1"/>
+        <v>2.1187791064193079E-2</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>44859</v>
       </c>
       <c r="B117">
         <v>248.787216</v>
       </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C117">
+        <f t="shared" si="1"/>
+        <v>1.3791702654284244E-2</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>44860</v>
       </c>
       <c r="B118">
         <v>229.59172100000001</v>
       </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C118">
+        <f t="shared" si="1"/>
+        <v>-7.7156275586121731E-2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>44861</v>
       </c>
       <c r="B119">
         <v>225.055847</v>
       </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C119">
+        <f t="shared" si="1"/>
+        <v>-1.9756261158911766E-2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>44862</v>
       </c>
       <c r="B120">
         <v>234.10771199999999</v>
       </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C120">
+        <f t="shared" si="1"/>
+        <v>4.022052801854107E-2</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>44865</v>
       </c>
       <c r="B121">
         <v>230.39565999999999</v>
       </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C121">
+        <f t="shared" si="1"/>
+        <v>-1.585617136781893E-2</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>44866</v>
       </c>
       <c r="B122">
         <v>226.46525600000001</v>
       </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C122">
+        <f t="shared" si="1"/>
+        <v>-1.7059366482858149E-2</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>44867</v>
       </c>
       <c r="B123">
         <v>218.45555100000001</v>
       </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C123">
+        <f t="shared" si="1"/>
+        <v>-3.5368361317199122E-2</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>44868</v>
       </c>
       <c r="B124">
         <v>212.649261</v>
       </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C124">
+        <f t="shared" si="1"/>
+        <v>-2.6578816484274268E-2</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>44869</v>
       </c>
       <c r="B125">
         <v>219.735916</v>
       </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C125">
+        <f t="shared" si="1"/>
+        <v>3.3325556678045577E-2</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>44872</v>
       </c>
       <c r="B126">
         <v>226.167496</v>
       </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C126">
+        <f t="shared" si="1"/>
+        <v>2.9269589228189698E-2</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>44873</v>
       </c>
       <c r="B127">
         <v>227.16001900000001</v>
       </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C127">
+        <f t="shared" si="1"/>
+        <v>4.3884422720053707E-3</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>44874</v>
       </c>
       <c r="B128">
         <v>222.832596</v>
       </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C128">
+        <f t="shared" si="1"/>
+        <v>-1.9050108461207735E-2</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>44875</v>
       </c>
       <c r="B129">
         <v>241.16459699999999</v>
       </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C129">
+        <f t="shared" si="1"/>
+        <v>8.2268040354383301E-2</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>44876</v>
       </c>
       <c r="B130">
         <v>245.26374799999999</v>
       </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C130">
+        <f t="shared" si="1"/>
+        <v>1.6997316567157684E-2</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>44879</v>
       </c>
       <c r="B131">
         <v>239.745285</v>
       </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C131">
+        <f t="shared" si="1"/>
+        <v>-2.2500116894568524E-2</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>44880</v>
       </c>
       <c r="B132">
         <v>240.16213999999999</v>
       </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C132">
+        <f t="shared" ref="C132:C162" si="2">(B132-B131)/B131</f>
+        <v>1.7387411810830741E-3</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>44881</v>
       </c>
       <c r="B133">
         <v>240.60008199999999</v>
       </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C133">
+        <f t="shared" si="2"/>
+        <v>1.8235263892967997E-3</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>44882</v>
       </c>
       <c r="B134">
         <v>240.550308</v>
       </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C134">
+        <f t="shared" si="2"/>
+        <v>-2.0687440995961553E-4</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>44883</v>
       </c>
       <c r="B135">
         <v>240.092468</v>
       </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C135">
+        <f t="shared" si="2"/>
+        <v>-1.9033024892240191E-3</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>44886</v>
       </c>
       <c r="B136">
         <v>240.91859400000001</v>
       </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C136">
+        <f t="shared" si="2"/>
+        <v>3.4408659583607445E-3</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>44887</v>
       </c>
       <c r="B137">
         <v>243.884659</v>
       </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C137">
+        <f t="shared" si="2"/>
+        <v>1.2311482276042115E-2</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>44888</v>
       </c>
       <c r="B138">
         <v>246.42274499999999</v>
       </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C138">
+        <f t="shared" si="2"/>
+        <v>1.040691124405653E-2</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>44890</v>
       </c>
       <c r="B139">
         <v>246.33315999999999</v>
       </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C139">
+        <f t="shared" si="2"/>
+        <v>-3.6354192872902044E-4</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>44893</v>
       </c>
       <c r="B140">
         <v>240.62994399999999</v>
       </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C140">
+        <f t="shared" si="2"/>
+        <v>-2.3152449308895311E-2</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>44894</v>
       </c>
       <c r="B141">
         <v>239.20663500000001</v>
       </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C141">
+        <f t="shared" si="2"/>
+        <v>-5.9149288585629602E-3</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>44895</v>
       </c>
       <c r="B142">
         <v>253.94740300000001</v>
       </c>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C142">
+        <f t="shared" si="2"/>
+        <v>6.1623574948077853E-2</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>44896</v>
       </c>
       <c r="B143">
         <v>253.49949599999999</v>
       </c>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C143">
+        <f t="shared" si="2"/>
+        <v>-1.7637786199373533E-3</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>44897</v>
       </c>
       <c r="B144">
         <v>253.827957</v>
       </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C144">
+        <f t="shared" si="2"/>
+        <v>1.2957067180914804E-3</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>44900</v>
       </c>
       <c r="B145">
         <v>249.03048699999999</v>
       </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C145">
+        <f t="shared" si="2"/>
+        <v>-1.8900479114678469E-2</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>44901</v>
       </c>
       <c r="B146">
         <v>243.97422800000001</v>
       </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C146">
+        <f t="shared" si="2"/>
+        <v>-2.0303775095617042E-2</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>44902</v>
       </c>
       <c r="B147">
         <v>243.22773699999999</v>
       </c>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C147">
+        <f t="shared" si="2"/>
+        <v>-3.0597125201274134E-3</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>44903</v>
       </c>
       <c r="B148">
         <v>246.24357599999999</v>
       </c>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C148">
+        <f t="shared" si="2"/>
+        <v>1.2399239647573581E-2</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>44904</v>
       </c>
       <c r="B149">
         <v>244.27282700000001</v>
       </c>
-    </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C149">
+        <f t="shared" si="2"/>
+        <v>-8.0032504076369641E-3</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>44907</v>
       </c>
       <c r="B150">
         <v>251.32968099999999</v>
       </c>
-    </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C150">
+        <f t="shared" si="2"/>
+        <v>2.8889230483257915E-2</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>44908</v>
       </c>
       <c r="B151">
         <v>255.719086</v>
       </c>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C151">
+        <f t="shared" si="2"/>
+        <v>1.7464729921811386E-2</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>44909</v>
       </c>
       <c r="B152">
         <v>256.01769999999999</v>
       </c>
-    </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C152">
+        <f t="shared" si="2"/>
+        <v>1.1677423248727958E-3</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>44910</v>
       </c>
       <c r="B153">
         <v>247.84605400000001</v>
       </c>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C153">
+        <f t="shared" si="2"/>
+        <v>-3.1918285337302781E-2</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>44911</v>
       </c>
       <c r="B154">
         <v>243.54624899999999</v>
       </c>
-    </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C154">
+        <f t="shared" si="2"/>
+        <v>-1.734869258802087E-2</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>44914</v>
       </c>
       <c r="B155">
         <v>239.326065</v>
       </c>
-    </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C155">
+        <f t="shared" si="2"/>
+        <v>-1.7328059936574877E-2</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>44915</v>
       </c>
       <c r="B156">
         <v>240.66975400000001</v>
       </c>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C156">
+        <f t="shared" si="2"/>
+        <v>5.6144699491884088E-3</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>44916</v>
       </c>
       <c r="B157">
         <v>243.28744499999999</v>
       </c>
-    </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C157">
+        <f t="shared" si="2"/>
+        <v>1.0876692880984036E-2</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>44917</v>
       </c>
       <c r="B158">
         <v>237.07662999999999</v>
       </c>
-    </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C158">
+        <f t="shared" si="2"/>
+        <v>-2.5528711520645862E-2</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>44918</v>
       </c>
       <c r="B159">
         <v>237.614105</v>
       </c>
-    </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C159">
+        <f t="shared" si="2"/>
+        <v>2.2670939771667945E-3</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>44922</v>
       </c>
       <c r="B160">
         <v>235.852386</v>
       </c>
-    </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C160">
+        <f t="shared" si="2"/>
+        <v>-7.4142021156530227E-3</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>44923</v>
       </c>
       <c r="B161">
         <v>233.43373099999999</v>
       </c>
-    </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C161">
+        <f t="shared" si="2"/>
+        <v>-1.0254952434528269E-2</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>44924</v>
       </c>
       <c r="B162">
         <v>239.88343800000001</v>
+      </c>
+      <c r="C162">
+        <f t="shared" si="2"/>
+        <v>2.7629713034060265E-2</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B163">
+        <v>239.45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>